<commit_message>
implemented 3d resnet and have written down linear and nonlinear model results
</commit_message>
<xml_diff>
--- a/Linear Model Results.xlsx
+++ b/Linear Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Portable\Documents\GitHub\CMPUT624_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54654BB-9EE1-4491-8EFB-09C4DD9B6FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0EB47D-BBA7-4AE0-A9A3-29B56DAB077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Inputs</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>2/3 folds, 500 epochs each, LR=1e-7, momentum=0.9</t>
+  </si>
+  <si>
+    <t>Model Details</t>
+  </si>
+  <si>
+    <t>Fully connect layer, no activations</t>
+  </si>
+  <si>
+    <t>1 fold, 1000 epochs, LR=1e-7, momentum=0.9</t>
+  </si>
+  <si>
+    <t>1 fold, 1000 epochs, LR=1e-3, momentum=0.9</t>
   </si>
 </sst>
 </file>
@@ -419,24 +431,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,230 +456,288 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2138.38</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1490.78</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.75290000000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.73740000000000006</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>2436.04</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1264.17</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.70750000000000002</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.6946</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1700.2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>958.81</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.83260000000000001</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.82909999999999995</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>2073.4699999999998</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1086.3</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.77539999999999998</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.77</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>222.29</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>114.02</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.73740000000000006</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.72030000000000005</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
         <v>195.02</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>103.96</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.78090000000000004</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.77470000000000006</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
         <v>163.11000000000001</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>100.47</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.84850000000000003</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.78790000000000004</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>20984.560000000001</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>14029.5</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.52910000000000001</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.51980000000000004</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>2869</v>
+      </c>
+      <c r="F10">
+        <v>1544</v>
+      </c>
+      <c r="G10">
+        <v>0.64</v>
+      </c>
+      <c r="H10">
+        <v>0.64</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1181</v>
+      </c>
+      <c r="F11">
+        <v>1098</v>
+      </c>
+      <c r="G11">
+        <v>0.88</v>
+      </c>
+      <c r="H11">
+        <v>0.79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>